<commit_message>
Updated plant scheme image and sizes
</commit_message>
<xml_diff>
--- a/translation-project/Assets/Images/cenario-vegetacao/esquema_plantas.xlsx
+++ b/translation-project/Assets/Images/cenario-vegetacao/esquema_plantas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\du0x\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\du0x\Desktop\antartica\testes-ferramentas\translation-project\Assets\Images\cenario-vegetacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -51,9 +51,6 @@
     <t>Possui flor?</t>
   </si>
   <si>
-    <t>NÃO                (POSSUI ESTRÓBILOS)</t>
-  </si>
-  <si>
     <t>Produz fruto?</t>
   </si>
   <si>
@@ -79,6 +76,10 @@
   </si>
   <si>
     <t>Raiz, caule, folhas, flores, sementes e frutos</t>
+  </si>
+  <si>
+    <t>NÃO 
+(POSSUI ESTRÓBILOS)</t>
   </si>
 </sst>
 </file>
@@ -492,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -501,8 +502,8 @@
     <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" style="1" customWidth="1"/>
     <col min="7" max="8" width="14.42578125" style="1"/>
     <col min="9" max="9" width="16.28515625" style="1" customWidth="1"/>
@@ -559,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -570,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
@@ -578,7 +579,7 @@
     </row>
     <row r="5" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>5</v>
@@ -595,24 +596,24 @@
     </row>
     <row r="6" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>6</v>
@@ -627,21 +628,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated text to sementes
</commit_message>
<xml_diff>
--- a/translation-project/Assets/Images/cenario-vegetacao/esquema_plantas.xlsx
+++ b/translation-project/Assets/Images/cenario-vegetacao/esquema_plantas.xlsx
@@ -72,14 +72,14 @@
     <t>Raiz, caule e folhas</t>
   </si>
   <si>
-    <t>Raiz, caule, folhas, estróbilos e semente</t>
-  </si>
-  <si>
     <t>Raiz, caule, folhas, flores, sementes e frutos</t>
   </si>
   <si>
     <t>NÃO 
 (POSSUI ESTRÓBILOS)</t>
+  </si>
+  <si>
+    <t>Raiz, caule, folhas, estróbilos e sementes</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -571,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>6</v>
@@ -639,10 +639,10 @@
         <v>16</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>